<commit_message>
A lot of progress!
</commit_message>
<xml_diff>
--- a/Player.xlsx
+++ b/Player.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Match" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -456,7 +456,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
SpringSecurity & FileUpload OK
</commit_message>
<xml_diff>
--- a/Player.xlsx
+++ b/Player.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Match" sheetId="1" r:id="rId1"/>
+    <sheet name="REPO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
   <si>
     <t>EMAIL_ADDRESS</t>
   </si>
@@ -92,6 +93,78 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Duran</t>
+  </si>
+  <si>
+    <t>kevind@yahoo.com</t>
+  </si>
+  <si>
+    <t>Golden States</t>
+  </si>
+  <si>
+    <t>Irving</t>
+  </si>
+  <si>
+    <t>Kyrie</t>
+  </si>
+  <si>
+    <t>Kirving@me.com</t>
+  </si>
+  <si>
+    <t>Boston Celtics</t>
+  </si>
+  <si>
+    <t>Point-guard</t>
+  </si>
+  <si>
+    <t>Shooting-guard</t>
+  </si>
+  <si>
+    <t>Luka</t>
+  </si>
+  <si>
+    <t>Doncic</t>
+  </si>
+  <si>
+    <t>Luka.doncic@myemail.com</t>
+  </si>
+  <si>
+    <t>Dallas Maverics</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>ROLES</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>abcdedfdf</t>
+  </si>
+  <si>
+    <t>1234ABcd</t>
+  </si>
+  <si>
+    <t>San</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>dsdsdsds@sas.com</t>
+  </si>
+  <si>
+    <t>938@fdfd.com</t>
   </si>
 </sst>
 </file>
@@ -142,12 +215,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -453,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -471,9 +546,10 @@
     <col min="8" max="8" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -504,8 +580,14 @@
       <c r="J1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -513,6 +595,190 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="4">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="3">
+        <v>30247</v>
+      </c>
+      <c r="H2" s="4">
+        <v>85</v>
+      </c>
+      <c r="I2" s="4">
+        <v>185</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3">
+        <v>30247</v>
+      </c>
+      <c r="H3" s="4">
+        <v>85</v>
+      </c>
+      <c r="I3" s="4">
+        <v>185</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="E4" s="4"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="E5" s="4"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="E6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
@@ -533,8 +799,14 @@
       <c r="J2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2">
+        <v>12345678</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -565,8 +837,14 @@
       <c r="J3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3">
+        <v>12345678</v>
+      </c>
+      <c r="L3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -596,6 +874,126 @@
       </c>
       <c r="J4" t="s">
         <v>25</v>
+      </c>
+      <c r="K4">
+        <v>12345678</v>
+      </c>
+      <c r="L4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="4">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3">
+        <v>29517</v>
+      </c>
+      <c r="H5" s="4">
+        <v>92</v>
+      </c>
+      <c r="I5" s="4">
+        <v>210</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5">
+        <v>12345678</v>
+      </c>
+      <c r="L5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="4">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="3">
+        <v>33686</v>
+      </c>
+      <c r="H6" s="4">
+        <v>82</v>
+      </c>
+      <c r="I6" s="4">
+        <v>191</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>12345678</v>
+      </c>
+      <c r="L6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="4">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3">
+        <v>36219</v>
+      </c>
+      <c r="H7" s="4">
+        <v>97</v>
+      </c>
+      <c r="I7" s="4">
+        <v>201</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7">
+        <v>12345678</v>
+      </c>
+      <c r="L7" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -603,8 +1001,10 @@
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>